<commit_message>
Use direct backend IP to bypass Traefik timeout issue
🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/relume_structure_web.xlsx
+++ b/relume_structure_web.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A37E54B-8AE9-44B9-8811-7805186B8484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD910B73-65AC-4E11-96A5-D4F70BBEEEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{E5AF001E-23D7-422A-B940-F5D63691E857}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E5AF001E-23D7-422A-B940-F5D63691E857}"/>
   </bookViews>
   <sheets>
     <sheet name="Estructura web" sheetId="1" r:id="rId1"/>
-    <sheet name="Estructura home" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,12 +30,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="132">
   <si>
     <t>Página</t>
   </si>
@@ -152,13 +155,292 @@
   </si>
   <si>
     <t>#093D53</t>
+  </si>
+  <si>
+    <t>Nosotros</t>
+  </si>
+  <si>
+    <t>servicios_hero</t>
+  </si>
+  <si>
+    <t>Header 114</t>
+  </si>
+  <si>
+    <t>servicios_origen</t>
+  </si>
+  <si>
+    <t>Header 141</t>
+  </si>
+  <si>
+    <t>servicios_vision</t>
+  </si>
+  <si>
+    <t>Layout 93</t>
+  </si>
+  <si>
+    <t>servicios_trayectoria</t>
+  </si>
+  <si>
+    <t>Timeline 20</t>
+  </si>
+  <si>
+    <t>servicios_voces</t>
+  </si>
+  <si>
+    <t>Layout 213</t>
+  </si>
+  <si>
+    <t>Logo 3</t>
+  </si>
+  <si>
+    <t>Scheme 3</t>
+  </si>
+  <si>
+    <t>servicios_logolist</t>
+  </si>
+  <si>
+    <t>servicios_cde</t>
+  </si>
+  <si>
+    <t>CTA 39</t>
+  </si>
+  <si>
+    <t>Schema 1</t>
+  </si>
+  <si>
+    <t>Worksys</t>
+  </si>
+  <si>
+    <t>worksys_hero</t>
+  </si>
+  <si>
+    <t>Header 30</t>
+  </si>
+  <si>
+    <t>worksys_description</t>
+  </si>
+  <si>
+    <t>Layout 421</t>
+  </si>
+  <si>
+    <t>Layout74</t>
+  </si>
+  <si>
+    <t>worksys_resultado</t>
+  </si>
+  <si>
+    <t>worksys_empresas</t>
+  </si>
+  <si>
+    <t>Layout 243</t>
+  </si>
+  <si>
+    <t>Layout 109</t>
+  </si>
+  <si>
+    <t>worksys_industrias</t>
+  </si>
+  <si>
+    <t>Layout 237</t>
+  </si>
+  <si>
+    <t>worksys_momentos</t>
+  </si>
+  <si>
+    <t>FAQ 3</t>
+  </si>
+  <si>
+    <t>worksys_momentos2</t>
+  </si>
+  <si>
+    <t>worksys_clientes</t>
+  </si>
+  <si>
+    <t>Worksys_cta</t>
+  </si>
+  <si>
+    <t>worksys_blog</t>
+  </si>
+  <si>
+    <t>Blog 37</t>
+  </si>
+  <si>
+    <t>worksys_faq</t>
+  </si>
+  <si>
+    <t>FAQ 5</t>
+  </si>
+  <si>
+    <t>expersys_hero</t>
+  </si>
+  <si>
+    <t>Expersys</t>
+  </si>
+  <si>
+    <t>Schema 2</t>
+  </si>
+  <si>
+    <t>expersys_features</t>
+  </si>
+  <si>
+    <t>Layout 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layout 492 </t>
+  </si>
+  <si>
+    <t>expersys_auditoria</t>
+  </si>
+  <si>
+    <t>expersys_stack</t>
+  </si>
+  <si>
+    <t>Layout 121</t>
+  </si>
+  <si>
+    <t>expersys_casos</t>
+  </si>
+  <si>
+    <t>Layout 253</t>
+  </si>
+  <si>
+    <t>expersys_exito</t>
+  </si>
+  <si>
+    <t>Layout 239</t>
+  </si>
+  <si>
+    <t>expersys_cta</t>
+  </si>
+  <si>
+    <t>expersys_faq</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>clientes_hero</t>
+  </si>
+  <si>
+    <t>Header 64</t>
+  </si>
+  <si>
+    <t>clientes_portfolio</t>
+  </si>
+  <si>
+    <t>Portfolio 9</t>
+  </si>
+  <si>
+    <t>clientes_blueprints</t>
+  </si>
+  <si>
+    <t>Event 23</t>
+  </si>
+  <si>
+    <t>Client-entry</t>
+  </si>
+  <si>
+    <t>awalab_inicio</t>
+  </si>
+  <si>
+    <t>Blog post Header 1</t>
+  </si>
+  <si>
+    <t>Content 27</t>
+  </si>
+  <si>
+    <t>awalab_indice</t>
+  </si>
+  <si>
+    <t>awalab_datos</t>
+  </si>
+  <si>
+    <t>Stats 30</t>
+  </si>
+  <si>
+    <t>awalab_testimonio</t>
+  </si>
+  <si>
+    <t>Testimonial 17</t>
+  </si>
+  <si>
+    <t>awalab_galeria</t>
+  </si>
+  <si>
+    <t>Gallery 1</t>
+  </si>
+  <si>
+    <t>awalab_cta</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>blog_galeria</t>
+  </si>
+  <si>
+    <t>Blog 30</t>
+  </si>
+  <si>
+    <t>blog_documentos</t>
+  </si>
+  <si>
+    <t>Blog 68</t>
+  </si>
+  <si>
+    <t>blog_contacto</t>
+  </si>
+  <si>
+    <t>Contact 13</t>
+  </si>
+  <si>
+    <t>Blog-entry</t>
+  </si>
+  <si>
+    <t>blog_entry_portada</t>
+  </si>
+  <si>
+    <t>Blog Post Header 4</t>
+  </si>
+  <si>
+    <t>blog_entry_desarrollo</t>
+  </si>
+  <si>
+    <t>blog_entry_galeria</t>
+  </si>
+  <si>
+    <t>blog_entry_documentos</t>
+  </si>
+  <si>
+    <t>Contacto</t>
+  </si>
+  <si>
+    <t>contacto_hero</t>
+  </si>
+  <si>
+    <t>contacto_form</t>
+  </si>
+  <si>
+    <t>Contact 6</t>
+  </si>
+  <si>
+    <t>contacto_informacion</t>
+  </si>
+  <si>
+    <t>contacto_sedes</t>
+  </si>
+  <si>
+    <t>Contact 26</t>
+  </si>
+  <si>
+    <t>Imagen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,16 +448,77 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -183,13 +526,125 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -506,180 +961,1449 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD5DAA5-F633-49B3-AD61-F14FA4F853BA}">
-  <dimension ref="A2:F9"/>
+  <dimension ref="A2:J58"/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.1796875" customWidth="1"/>
-    <col min="4" max="4" width="24.08984375" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="G2" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+    </row>
+    <row r="3" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+    </row>
+    <row r="5" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+    </row>
+    <row r="6" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+    </row>
+    <row r="8" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+    </row>
+    <row r="9" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+    </row>
+    <row r="11" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+    </row>
+    <row r="12" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+    </row>
+    <row r="17" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+    </row>
+    <row r="19" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+    </row>
+    <row r="20" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+    </row>
+    <row r="21" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+    </row>
+    <row r="22" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+    </row>
+    <row r="23" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+    </row>
+    <row r="25" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+    </row>
+    <row r="26" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+    </row>
+    <row r="27" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>25</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+    </row>
+    <row r="28" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+    </row>
+    <row r="29" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+    </row>
+    <row r="30" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+    </row>
+    <row r="31" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+    </row>
+    <row r="32" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>31</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+    </row>
+    <row r="34" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+    </row>
+    <row r="35" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+    </row>
+    <row r="36" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+    </row>
+    <row r="37" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+    </row>
+    <row r="38" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+    </row>
+    <row r="39" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+    </row>
+    <row r="40" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+    </row>
+    <row r="41" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+    </row>
+    <row r="42" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>40</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+    </row>
+    <row r="43" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>41</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+    </row>
+    <row r="44" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+    </row>
+    <row r="45" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>43</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+    </row>
+    <row r="46" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+    </row>
+    <row r="47" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6">
+        <v>45</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+    </row>
+    <row r="48" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="6">
+        <v>46</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+    </row>
+    <row r="49" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>47</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+    </row>
+    <row r="50" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6">
+        <v>48</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+    </row>
+    <row r="51" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6">
+        <v>49</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+    </row>
+    <row r="52" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>50</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+    </row>
+    <row r="53" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>51</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+    </row>
+    <row r="54" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>52</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+    </row>
+    <row r="55" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>53</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="21"/>
+    </row>
+    <row r="56" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>54</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+    </row>
+    <row r="57" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>55</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+    </row>
+    <row r="58" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>56</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
     </row>
   </sheetData>
+  <mergeCells count="57">
+    <mergeCell ref="G56:J56"/>
+    <mergeCell ref="G57:J57"/>
+    <mergeCell ref="G58:J58"/>
+    <mergeCell ref="G50:J50"/>
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="G52:J52"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="G54:J54"/>
+    <mergeCell ref="G55:J55"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="G45:J45"/>
+    <mergeCell ref="G46:J46"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="G49:J49"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="G43:J43"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G7:J7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -688,16 +2412,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D562D4B1-9106-4E24-9965-CAB89C52D85B}">
   <dimension ref="B2:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
@@ -717,7 +2441,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -737,7 +2461,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -757,7 +2481,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -777,7 +2501,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>4</v>
       </c>

</xml_diff>